<commit_message>
novas aulas credit scoring
</commit_message>
<xml_diff>
--- a/fia/provas/20210701/Teste-de-Hipotese Modificado.xlsx
+++ b/fia/provas/20210701/Teste-de-Hipotese Modificado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\github.com\datascience\fia\provas\20210701\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C52D9A-5223-4C3F-ABA4-408BFAC0B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D85B33E-F19F-4390-A1FE-552E782E2F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="749" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-465" windowWidth="29040" windowHeight="15990" tabRatio="749" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intervalo_Confiança=&gt;" sheetId="25" r:id="rId1"/>
@@ -7321,7 +7321,7 @@
   <dimension ref="B1:N8"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7362,14 +7362,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="18">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="16">
         <f>C4*(C6/SQRT(C5))</f>
-        <v>2323.6808465476311</v>
+        <v>1.6630845892196129</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="15.75">
@@ -7378,18 +7378,18 @@
       </c>
       <c r="C4" s="54">
         <f>NORMSINV(C3+((1-C3)/2))</f>
-        <v>2.5758293035488999</v>
+        <v>1.9599639845400536</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="17">
         <f>C7-F3</f>
-        <v>21076.319153452368</v>
+        <v>23398.336915410779</v>
       </c>
       <c r="K4" s="17">
         <f>C7+F3</f>
-        <v>25723.680846547632</v>
+        <v>23401.663084589221</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>4</v>
@@ -7403,7 +7403,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>7</v>
@@ -7414,7 +7414,7 @@
         <v>51</v>
       </c>
       <c r="C6" s="2">
-        <v>6250</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="15.75">
@@ -7446,7 +7446,7 @@
   <dimension ref="B1:N8"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7486,14 +7486,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="18">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="16">
         <f>C4*(C6/SQRT(C5))</f>
-        <v>77.496445431487984</v>
+        <v>0.40722105871397268</v>
       </c>
     </row>
     <row r="4" spans="2:14">
@@ -7502,18 +7502,18 @@
       </c>
       <c r="C4" s="54">
         <f>_xlfn.T.INV(C3+((1-C3)/2),C5-1)</f>
-        <v>2.6845556178665237</v>
+        <v>1.6456255198576413</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="17">
         <f>C7-F3</f>
-        <v>23322.503554568513</v>
+        <v>27.592778941286028</v>
       </c>
       <c r="K4" s="17">
         <f>C7+F3</f>
-        <v>23477.496445431487</v>
+        <v>28.407221058713972</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>4</v>
@@ -7527,7 +7527,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="2">
-        <v>48</v>
+        <v>1976</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>7</v>
@@ -7538,7 +7538,7 @@
         <v>51</v>
       </c>
       <c r="C6" s="2">
-        <v>200</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:14">
@@ -7546,7 +7546,7 @@
         <v>35</v>
       </c>
       <c r="C7" s="2">
-        <v>23400</v>
+        <v>28</v>
       </c>
       <c r="J7" s="11"/>
     </row>
@@ -7730,8 +7730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:T9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7827,12 +7827,14 @@
         <v>39</v>
       </c>
       <c r="O3" s="2">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="Q3" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="2"/>
+      <c r="R3" s="2">
+        <v>110</v>
+      </c>
     </row>
     <row r="4" spans="2:20">
       <c r="B4" s="42" t="s">
@@ -7869,14 +7871,14 @@
       </c>
       <c r="O4" s="48">
         <f>1-O3</f>
-        <v>1.0000000000000009E-2</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="Q4" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="16" t="e">
+      <c r="R4" s="16">
         <f>(R3-O8)/(O7/(SQRT(O6)))</f>
-        <v>#DIV/0!</v>
+        <v>-2.7386127875258306</v>
       </c>
     </row>
     <row r="5" spans="2:20">
@@ -7914,14 +7916,14 @@
       </c>
       <c r="O5" s="54">
         <f>NORMSINV(O3)</f>
-        <v>2.3263478740408408</v>
+        <v>1.2815515655446006</v>
       </c>
       <c r="Q5" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="R5" s="53" t="e">
+      <c r="R5" s="53">
         <f>_xlfn.NORM.S.DIST(R4, TRUE)</f>
-        <v>#DIV/0!</v>
+        <v>3.0849496602720801E-3</v>
       </c>
     </row>
     <row r="6" spans="2:20">
@@ -7970,7 +7972,9 @@
       <c r="N7" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>20</v>
+      </c>
       <c r="T7" s="10" t="s">
         <v>7</v>
       </c>
@@ -7991,7 +7995,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="2">
-        <v>1050</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:20">
@@ -8018,7 +8022,7 @@
   <dimension ref="B1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8318,7 +8322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>

</xml_diff>